<commit_message>
Add DateTimeTest test cases
</commit_message>
<xml_diff>
--- a/DateTimeTest/DateTimeTest.xlsx
+++ b/DateTimeTest/DateTimeTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brion/Sync/laravel-excel-seeder-test-data/DateTimeTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B8905-390B-DB49-9079-C2D55CF20067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2109CE-2544-C549-B549-1D2347FB0186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32520" yWindow="2160" windowWidth="25640" windowHeight="14440" xr2:uid="{CAE7E44F-FE30-3041-A7FB-011D23E69F8D}"/>
+    <workbookView xWindow="-32020" yWindow="500" windowWidth="27300" windowHeight="21040" xr2:uid="{CAE7E44F-FE30-3041-A7FB-011D23E69F8D}"/>
   </bookViews>
   <sheets>
     <sheet name="date_time_test" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>2020-10-04 05:31:02.440000000</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>10/15/2020</t>
+  </si>
+  <si>
+    <t>empty cells</t>
+  </si>
+  <si>
+    <t>explicit null cells</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -64,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -417,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E4A884-3F38-C940-A973-10092768EAB2}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,7 +444,7 @@
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -448,8 +460,11 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -464,6 +479,37 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add EmptyValueTest test data Update DateTimeTest with default value
</commit_message>
<xml_diff>
--- a/DateTimeTest/DateTimeTest.xlsx
+++ b/DateTimeTest/DateTimeTest.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brion/Sync/laravel-excel-seeder-test-data/DateTimeTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brion/development/laravel-excel-seeder/laravel-excel-seeder-test-data/DateTimeTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2109CE-2544-C549-B549-1D2347FB0186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB29C131-B532-C94C-9CA4-3B7BD3680459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32020" yWindow="500" windowWidth="27300" windowHeight="21040" xr2:uid="{CAE7E44F-FE30-3041-A7FB-011D23E69F8D}"/>
   </bookViews>
   <sheets>
     <sheet name="date_time_test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>2020-10-04 05:31:02.440000000</t>
   </si>
@@ -69,6 +72,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>default_value</t>
   </si>
 </sst>
 </file>
@@ -107,10 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -133,9 +138,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +178,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -279,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,7 +426,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E4A884-3F38-C940-A973-10092768EAB2}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,9 +447,10 @@
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -461,17 +467,20 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>44119.984027777777</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1602823029</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -480,19 +489,20 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -509,10 +519,14 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>